<commit_message>
Patched a bug in v0.9.0 related to Tf collection.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_full.xlsx
+++ b/andes/cases/kundur/kundur_full.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/notebooks/kundur/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E127581F-5E67-6C47-9921-0F29AE3B4CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="460" windowWidth="31900" windowHeight="19340" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -20,16 +14,16 @@
     <sheet name="Line" sheetId="5" r:id="rId5"/>
     <sheet name="Area" sheetId="6" r:id="rId6"/>
     <sheet name="GENROU" sheetId="7" r:id="rId7"/>
-    <sheet name="TGOV1" sheetId="9" r:id="rId8"/>
-    <sheet name="EXDC2" sheetId="10" r:id="rId9"/>
-    <sheet name="Toggler" sheetId="8" r:id="rId10"/>
+    <sheet name="TGOV1" sheetId="8" r:id="rId8"/>
+    <sheet name="EXDC2" sheetId="9" r:id="rId9"/>
+    <sheet name="Toggler" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="119">
   <si>
     <t>idx</t>
   </si>
@@ -280,6 +274,99 @@
     <t>GENROU_4</t>
   </si>
   <si>
+    <t>syn</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>wref0</t>
+  </si>
+  <si>
+    <t>VMAX</t>
+  </si>
+  <si>
+    <t>VMIN</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>Dt</t>
+  </si>
+  <si>
+    <t>TGOV1_1</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>TF1</t>
+  </si>
+  <si>
+    <t>KF1</t>
+  </si>
+  <si>
+    <t>KA</t>
+  </si>
+  <si>
+    <t>KE</t>
+  </si>
+  <si>
+    <t>VRMAX</t>
+  </si>
+  <si>
+    <t>VRMIN</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>SE1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>SE2</t>
+  </si>
+  <si>
+    <t>Ae</t>
+  </si>
+  <si>
+    <t>Be</t>
+  </si>
+  <si>
+    <t>EXDC2_1</t>
+  </si>
+  <si>
+    <t>EXDC2_2</t>
+  </si>
+  <si>
+    <t>EXDC2_3</t>
+  </si>
+  <si>
+    <t>EXDC2_4</t>
+  </si>
+  <si>
     <t>model</t>
   </si>
   <si>
@@ -293,106 +380,13 @@
   </si>
   <si>
     <t>Line</t>
-  </si>
-  <si>
-    <t>syn</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>wref0</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>TGOV1_1</t>
-  </si>
-  <si>
-    <t>Ae</t>
-  </si>
-  <si>
-    <t>Be</t>
-  </si>
-  <si>
-    <t>EXDC2_1</t>
-  </si>
-  <si>
-    <t>EXDC2_2</t>
-  </si>
-  <si>
-    <t>EXDC2_3</t>
-  </si>
-  <si>
-    <t>EXDC2_4</t>
-  </si>
-  <si>
-    <t>Dt</t>
-  </si>
-  <si>
-    <t>TR</t>
-  </si>
-  <si>
-    <t>TA</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>TB</t>
-  </si>
-  <si>
-    <t>TE</t>
-  </si>
-  <si>
-    <t>KF1</t>
-  </si>
-  <si>
-    <t>TF1</t>
-  </si>
-  <si>
-    <t>KA</t>
-  </si>
-  <si>
-    <t>KE</t>
-  </si>
-  <si>
-    <t>VRMAX</t>
-  </si>
-  <si>
-    <t>VRMIN</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>SE1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>SE2</t>
-  </si>
-  <si>
-    <t>VMIN</t>
-  </si>
-  <si>
-    <t>VMAX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,13 +402,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -424,7 +411,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -447,44 +434,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -531,7 +495,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -563,27 +527,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,24 +561,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -808,17 +736,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -862,7 +790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -879,7 +807,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G2">
         <v>0.9</v>
@@ -888,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.57025491716260168</v>
+        <v>0.5702549171626017</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -906,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -923,7 +851,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G3">
         <v>0.9</v>
@@ -932,7 +860,7 @@
         <v>0.99761</v>
       </c>
       <c r="I3">
-        <v>0.36874618304434781</v>
+        <v>0.3687461830443478</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -950,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -967,16 +895,16 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G4">
         <v>0.9</v>
       </c>
       <c r="H4">
-        <v>0.96262999999999999</v>
+        <v>0.96263</v>
       </c>
       <c r="I4">
-        <v>0.18531731464750281</v>
+        <v>0.1853173146475028</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -994,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1011,16 +939,16 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G5">
         <v>0.9</v>
       </c>
       <c r="H5">
-        <v>0.81691000000000003</v>
+        <v>0.81691</v>
       </c>
       <c r="I5">
-        <v>0.46235866280431398</v>
+        <v>0.462358662804314</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1038,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1055,16 +983,16 @@
         <v>230</v>
       </c>
       <c r="F6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6">
-        <v>0.97928000000000004</v>
+        <v>0.97928</v>
       </c>
       <c r="I6">
-        <v>0.48020290907670382</v>
+        <v>0.4802029090767038</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1082,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1099,16 +1027,16 @@
         <v>230</v>
       </c>
       <c r="F7">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G7">
         <v>0.9</v>
       </c>
       <c r="H7">
-        <v>0.95796000000000003</v>
+        <v>0.95796</v>
       </c>
       <c r="I7">
-        <v>0.28388652948313292</v>
+        <v>0.2838865294831329</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1126,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1143,16 +1071,16 @@
         <v>230</v>
       </c>
       <c r="F8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G8">
         <v>0.9</v>
       </c>
       <c r="H8">
-        <v>0.93620000000000003</v>
+        <v>0.9362</v>
       </c>
       <c r="I8">
-        <v>0.12690114458325361</v>
+        <v>0.1269011445832536</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1170,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1187,16 +1115,16 @@
         <v>230</v>
       </c>
       <c r="F9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G9">
         <v>0.9</v>
       </c>
       <c r="H9">
-        <v>0.87904000000000004</v>
+        <v>0.87904</v>
       </c>
       <c r="I9">
-        <v>-8.0592323540088801E-2</v>
+        <v>-0.0805923235400888</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1214,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1231,7 +1159,7 @@
         <v>230</v>
       </c>
       <c r="F10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G10">
         <v>0.9</v>
@@ -1240,7 +1168,7 @@
         <v>0.89054</v>
       </c>
       <c r="I10">
-        <v>9.3617715747722263E-2</v>
+        <v>0.09361771574772226</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1258,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1275,16 +1203,16 @@
         <v>230</v>
       </c>
       <c r="F11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G11">
         <v>0.9</v>
       </c>
       <c r="H11">
-        <v>0.82957999999999998</v>
+        <v>0.82958</v>
       </c>
       <c r="I11">
-        <v>0.33660070888111671</v>
+        <v>0.3366007088811167</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1308,17 +1236,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1332,16 +1260,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1352,10 +1280,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
@@ -1370,7 +1298,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1378,9 +1306,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1415,7 +1343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1435,10 +1363,10 @@
         <v>11.59</v>
       </c>
       <c r="H2">
-        <v>-0.73499999999999999</v>
+        <v>-0.735</v>
       </c>
       <c r="I2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J2">
         <v>0.9</v>
@@ -1447,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1467,10 +1395,10 @@
         <v>15.75</v>
       </c>
       <c r="H3">
-        <v>-0.89900000000000002</v>
+        <v>-0.899</v>
       </c>
       <c r="I3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J3">
         <v>0.9</v>
@@ -1485,7 +1413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1493,9 +1421,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1482,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1607,7 +1535,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1660,7 +1588,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1719,7 +1647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1727,9 +1655,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1791,7 +1719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1811,10 +1739,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.4586100000000002</v>
+        <v>7.45861</v>
       </c>
       <c r="J2">
-        <v>1.4361200000000001</v>
+        <v>1.43612</v>
       </c>
       <c r="K2">
         <v>9</v>
@@ -1844,7 +1772,7 @@
         <v>0.25</v>
       </c>
       <c r="T2">
-        <v>0.57025491716260168</v>
+        <v>0.5702549171626017</v>
       </c>
     </row>
   </sheetData>
@@ -1853,17 +1781,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1937,7 +1865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1966,13 +1894,13 @@
         <v>230</v>
       </c>
       <c r="K2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L2">
         <v>0.05</v>
       </c>
       <c r="M2">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1999,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2028,13 +1956,13 @@
         <v>230</v>
       </c>
       <c r="K3">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L3">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M3">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2061,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2090,7 +2018,7 @@
         <v>230</v>
       </c>
       <c r="K4">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L4">
         <v>0.02</v>
@@ -2123,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2152,10 +2080,10 @@
         <v>230</v>
       </c>
       <c r="K5">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L5">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -2185,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2214,10 +2142,10 @@
         <v>230</v>
       </c>
       <c r="K6">
-        <v>2.2009999999999998E-2</v>
+        <v>0.02201</v>
       </c>
       <c r="L6">
-        <v>0.22001000000000001</v>
+        <v>0.22001</v>
       </c>
       <c r="M6">
         <v>0.33</v>
@@ -2247,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2276,10 +2204,10 @@
         <v>230</v>
       </c>
       <c r="K7">
-        <v>2.2020000000000001E-2</v>
+        <v>0.02202</v>
       </c>
       <c r="L7">
-        <v>0.22001999999999999</v>
+        <v>0.22002</v>
       </c>
       <c r="M7">
         <v>0.33</v>
@@ -2309,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2338,7 +2266,7 @@
         <v>230</v>
       </c>
       <c r="K8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="L8">
         <v>0.22</v>
@@ -2371,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2400,7 +2328,7 @@
         <v>230</v>
       </c>
       <c r="K9">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L9">
         <v>0.02</v>
@@ -2433,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2462,10 +2390,10 @@
         <v>230</v>
       </c>
       <c r="K10">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L10">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M10">
         <v>0.03</v>
@@ -2495,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2524,13 +2452,13 @@
         <v>230</v>
       </c>
       <c r="K11">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L11">
         <v>0.05</v>
       </c>
       <c r="M11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2557,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2586,13 +2514,13 @@
         <v>230</v>
       </c>
       <c r="K12">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L12">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M12">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -2619,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2648,10 +2576,10 @@
         <v>230</v>
       </c>
       <c r="K13">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L13">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2681,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2710,10 +2638,10 @@
         <v>230</v>
       </c>
       <c r="K14">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L14">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -2743,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2772,10 +2700,10 @@
         <v>230</v>
       </c>
       <c r="K15">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L15">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -2805,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2834,10 +2762,10 @@
         <v>230</v>
       </c>
       <c r="K16">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2873,7 +2801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2881,9 +2809,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2897,7 +2825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2911,7 +2839,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2931,17 +2859,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V40" sqref="V40"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3027,7 +2955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3092,7 +3020,7 @@
         <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X2">
         <v>0.25</v>
@@ -3110,7 +3038,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3175,7 +3103,7 @@
         <v>0.25</v>
       </c>
       <c r="W3">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X3">
         <v>0.25</v>
@@ -3193,7 +3121,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3258,7 +3186,7 @@
         <v>0.25</v>
       </c>
       <c r="W4">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X4">
         <v>0.25</v>
@@ -3276,7 +3204,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3341,7 +3269,7 @@
         <v>0.25</v>
       </c>
       <c r="W5">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X5">
         <v>0.25</v>
@@ -3365,202 +3293,218 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>92</v>
       </c>
-      <c r="K1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>0.05</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>33</v>
       </c>
       <c r="I2">
+        <v>0.4</v>
+      </c>
+      <c r="J2">
         <v>0.49</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2.1</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>7</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>0</v>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.05</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
       <c r="G3">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>33</v>
       </c>
       <c r="I3">
+        <v>0.4</v>
+      </c>
+      <c r="J3">
         <v>0.49</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2.1</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>7</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0</v>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.05</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
       <c r="G4">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>33</v>
       </c>
       <c r="I4">
+        <v>0.4</v>
+      </c>
+      <c r="J4">
         <v>0.49</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2.1</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>7</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>0</v>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.05</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
       <c r="G5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>33</v>
       </c>
       <c r="I5">
+        <v>0.4</v>
+      </c>
+      <c r="J5">
         <v>0.49</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2.1</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>7</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0</v>
       </c>
     </row>
@@ -3570,17 +3514,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V2" sqref="V2:V5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3594,72 +3538,72 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>110</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3683,7 +3627,7 @@
         <v>1.246</v>
       </c>
       <c r="L2">
-        <v>7.5399999999999995E-2</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -3709,15 +3653,15 @@
       <c r="T2">
         <v>0</v>
       </c>
-      <c r="U2" s="3">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
@@ -3727,7 +3671,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3751,7 +3695,7 @@
         <v>1.246</v>
       </c>
       <c r="L3">
-        <v>7.5399999999999995E-2</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -3777,15 +3721,15 @@
       <c r="T3">
         <v>0</v>
       </c>
-      <c r="U3" s="3">
-        <v>0</v>
-      </c>
-      <c r="V3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
@@ -3795,7 +3739,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3819,7 +3763,7 @@
         <v>1.246</v>
       </c>
       <c r="L4">
-        <v>7.5399999999999995E-2</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="M4">
         <v>20</v>
@@ -3845,15 +3789,15 @@
       <c r="T4">
         <v>0</v>
       </c>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
@@ -3863,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -3887,7 +3831,7 @@
         <v>1.246</v>
       </c>
       <c r="L5">
-        <v>7.5399999999999995E-2</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="M5">
         <v>20</v>
@@ -3913,10 +3857,10 @@
       <c r="T5">
         <v>0</v>
       </c>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
         <v>0</v>
       </c>
     </row>

</xml_diff>